<commit_message>
Updated CHE model - 2025-09-06 17:10
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/Sets-vervestacks.xlsx
+++ b/VerveStacks_CHE/Sets-vervestacks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr updateLinks="never" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45088BA-E355-4D59-B6D8-AA94E14D9181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52485F27-B929-4917-B544-8B3D23B3A785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="98">
   <si>
     <t>~TFM_Psets</t>
   </si>
@@ -111,223 +111,226 @@
     <t>ep_gas_steam_turbine*,ep_oil_steam_turbine*</t>
   </si>
   <si>
+    <t>STG</t>
+  </si>
+  <si>
+    <t>*hydro*</t>
+  </si>
+  <si>
+    <t>Hydro pumped stg</t>
+  </si>
+  <si>
+    <t>IGCC</t>
+  </si>
+  <si>
+    <t>ep_bioenergy*,bioen*</t>
+  </si>
+  <si>
+    <t>ep_gas_combined_cycle*,ep_oil_combined_cycle*,CCGT*,*GasCC*</t>
+  </si>
+  <si>
+    <t>ep_gas_gas_turbine*,ep_oil_gas_turbine*,gas turbine*,EN*CT*</t>
+  </si>
+  <si>
+    <t>ep_coal_CFB*,ep_coal_subcritical*,*subcritical*</t>
+  </si>
+  <si>
+    <t>*IGCC*</t>
+  </si>
+  <si>
+    <t>ep_coal_supercritical*,ep_coal_supercritical_CCS*,ep_coal_ultra-supercritical*,ep_coal_ultra-supercritical_CCS*,*supercritical*</t>
+  </si>
+  <si>
+    <t>Gas_Oil Steam</t>
+  </si>
+  <si>
+    <t>Int Comb</t>
+  </si>
+  <si>
+    <t>EN*STG?hb*,-*EV*</t>
+  </si>
+  <si>
+    <t>Util Batt Stg</t>
+  </si>
+  <si>
+    <t>*EV*</t>
+  </si>
+  <si>
+    <t>EV Batt</t>
+  </si>
+  <si>
+    <t>solar</t>
+  </si>
+  <si>
+    <t>geothermal</t>
+  </si>
+  <si>
+    <t>hydro</t>
+  </si>
+  <si>
+    <t>nuclear</t>
+  </si>
+  <si>
+    <t>And</t>
+  </si>
+  <si>
+    <t>Or</t>
+  </si>
+  <si>
+    <t>Grid</t>
+  </si>
+  <si>
+    <t>IRE</t>
+  </si>
+  <si>
+    <t>g[_]*</t>
+  </si>
+  <si>
+    <t>DMD</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>e*spv*</t>
+  </si>
+  <si>
+    <t>e*won*,e*wof*</t>
+  </si>
+  <si>
+    <t>bioenergy</t>
+  </si>
+  <si>
+    <t>hydrogen</t>
+  </si>
+  <si>
+    <t>ELC</t>
+  </si>
+  <si>
+    <t>elc_buildings</t>
+  </si>
+  <si>
+    <t>elc_industry</t>
+  </si>
+  <si>
+    <t>elc_transport</t>
+  </si>
+  <si>
+    <t>elc_roadtransport</t>
+  </si>
+  <si>
+    <t>co2</t>
+  </si>
+  <si>
+    <t>co2captured</t>
+  </si>
+  <si>
+    <t>buildings</t>
+  </si>
+  <si>
+    <t>industry</t>
+  </si>
+  <si>
+    <t>transport</t>
+  </si>
+  <si>
+    <t>EVs</t>
+  </si>
+  <si>
+    <t>fossil</t>
+  </si>
+  <si>
+    <t>coal,gas,oil</t>
+  </si>
+  <si>
+    <t>geothermal,hydro,solar,wind</t>
+  </si>
+  <si>
+    <t>PRE</t>
+  </si>
+  <si>
+    <t>stepdown*</t>
+  </si>
+  <si>
+    <t>Nuclear P</t>
+  </si>
+  <si>
+    <t>*ror*</t>
+  </si>
+  <si>
+    <t>Hydro RoR</t>
+  </si>
+  <si>
+    <t>Geothermal P</t>
+  </si>
+  <si>
+    <t>Bio Power</t>
+  </si>
+  <si>
+    <t>Nuclear SMR</t>
+  </si>
+  <si>
+    <t>*SMR*</t>
+  </si>
+  <si>
+    <t>Solar Util</t>
+  </si>
+  <si>
+    <t>-*SMR*</t>
+  </si>
+  <si>
+    <t>-*ror*</t>
+  </si>
+  <si>
+    <t>Hydro Dam</t>
+  </si>
+  <si>
+    <t>renewable</t>
+  </si>
+  <si>
+    <t>Solar elec</t>
+  </si>
+  <si>
+    <t>Wind elec</t>
+  </si>
+  <si>
+    <t>Aggregators</t>
+  </si>
+  <si>
+    <t>IMP*Z</t>
+  </si>
+  <si>
+    <t>DUMMY_IMP</t>
+  </si>
+  <si>
+    <t>stepup*</t>
+  </si>
+  <si>
+    <t>Transformers Up</t>
+  </si>
+  <si>
+    <t>Transformers Dn</t>
+  </si>
+  <si>
+    <t>windon</t>
+  </si>
+  <si>
+    <t>windoff</t>
+  </si>
+  <si>
+    <t>Onshore Wind</t>
+  </si>
+  <si>
+    <t>Offshore Wind</t>
+  </si>
+  <si>
     <t>Wind onshore</t>
   </si>
   <si>
     <t>Wind offshore</t>
   </si>
   <si>
-    <t>-*WOF*</t>
-  </si>
-  <si>
-    <t>*WOF*</t>
-  </si>
-  <si>
-    <t>STG</t>
-  </si>
-  <si>
-    <t>*hydro*</t>
-  </si>
-  <si>
-    <t>Hydro pumped stg</t>
-  </si>
-  <si>
-    <t>IGCC</t>
-  </si>
-  <si>
-    <t>ep_bioenergy*,bioen*</t>
-  </si>
-  <si>
-    <t>ep_gas_combined_cycle*,ep_oil_combined_cycle*,CCGT*,*GasCC*</t>
-  </si>
-  <si>
-    <t>ep_gas_gas_turbine*,ep_oil_gas_turbine*,gas turbine*,EN*CT*</t>
-  </si>
-  <si>
-    <t>ep_coal_CFB*,ep_coal_subcritical*,*subcritical*</t>
-  </si>
-  <si>
-    <t>*IGCC*</t>
-  </si>
-  <si>
-    <t>ep_coal_supercritical*,ep_coal_supercritical_CCS*,ep_coal_ultra-supercritical*,ep_coal_ultra-supercritical_CCS*,*supercritical*</t>
-  </si>
-  <si>
-    <t>Gas_Oil Steam</t>
-  </si>
-  <si>
-    <t>Int Comb</t>
-  </si>
-  <si>
-    <t>EN*STG?hb*,-*EV*</t>
-  </si>
-  <si>
-    <t>Util Batt Stg</t>
-  </si>
-  <si>
-    <t>*EV*</t>
-  </si>
-  <si>
-    <t>EV Batt</t>
-  </si>
-  <si>
-    <t>solar</t>
-  </si>
-  <si>
-    <t>wind</t>
-  </si>
-  <si>
-    <t>geothermal</t>
-  </si>
-  <si>
-    <t>hydro</t>
-  </si>
-  <si>
-    <t>nuclear</t>
-  </si>
-  <si>
-    <t>And</t>
-  </si>
-  <si>
-    <t>Or</t>
-  </si>
-  <si>
-    <t>Grid</t>
-  </si>
-  <si>
-    <t>IRE</t>
-  </si>
-  <si>
-    <t>g[_]*</t>
-  </si>
-  <si>
-    <t>DMD</t>
-  </si>
-  <si>
-    <t>Demand</t>
-  </si>
-  <si>
-    <t>e*spv*</t>
-  </si>
-  <si>
-    <t>e*won*,e*wof*</t>
-  </si>
-  <si>
-    <t>bioenergy</t>
-  </si>
-  <si>
-    <t>hydrogen</t>
-  </si>
-  <si>
-    <t>ELC</t>
-  </si>
-  <si>
-    <t>elc_buildings</t>
-  </si>
-  <si>
-    <t>elc_industry</t>
-  </si>
-  <si>
-    <t>elc_transport</t>
-  </si>
-  <si>
-    <t>elc_roadtransport</t>
-  </si>
-  <si>
-    <t>co2</t>
-  </si>
-  <si>
-    <t>co2captured</t>
-  </si>
-  <si>
-    <t>buildings</t>
-  </si>
-  <si>
-    <t>industry</t>
-  </si>
-  <si>
-    <t>transport</t>
-  </si>
-  <si>
-    <t>EVs</t>
-  </si>
-  <si>
-    <t>fossil</t>
-  </si>
-  <si>
-    <t>coal,gas,oil</t>
-  </si>
-  <si>
-    <t>geothermal,hydro,solar,wind</t>
-  </si>
-  <si>
-    <t>PRE</t>
-  </si>
-  <si>
-    <t>stepdown*</t>
-  </si>
-  <si>
-    <t>Nuclear P</t>
-  </si>
-  <si>
-    <t>*ror*</t>
-  </si>
-  <si>
-    <t>Hydro RoR</t>
-  </si>
-  <si>
-    <t>Geothermal P</t>
-  </si>
-  <si>
-    <t>Bio Power</t>
-  </si>
-  <si>
-    <t>Nuclear SMR</t>
-  </si>
-  <si>
-    <t>*SMR*</t>
-  </si>
-  <si>
-    <t>Solar Util</t>
-  </si>
-  <si>
-    <t>-*SMR*</t>
-  </si>
-  <si>
-    <t>-*ror*</t>
-  </si>
-  <si>
-    <t>Hydro Dam</t>
-  </si>
-  <si>
-    <t>renewable</t>
-  </si>
-  <si>
-    <t>Solar elec</t>
-  </si>
-  <si>
-    <t>Wind elec</t>
-  </si>
-  <si>
     <t>distr*</t>
-  </si>
-  <si>
-    <t>Aggregators</t>
-  </si>
-  <si>
-    <t>IMP*Z</t>
-  </si>
-  <si>
-    <t>DUMMY_IMP</t>
-  </si>
-  <si>
-    <t>stepup*</t>
-  </si>
-  <si>
-    <t>Transformers Up</t>
-  </si>
-  <si>
-    <t>Transformers Dn</t>
   </si>
 </sst>
 </file>
@@ -723,7 +726,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1045,39 +1048,39 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D26" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D28" t="str">
         <f>B28</f>
@@ -1086,7 +1089,7 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D29" t="str">
         <f>B29</f>
@@ -1095,7 +1098,7 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D30" t="str">
         <f>B30</f>
@@ -1104,7 +1107,7 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D31" t="str">
         <f>B31</f>
@@ -1113,39 +1116,39 @@
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D32" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D33" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D34" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B35" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D36" t="str">
         <f>B36</f>
@@ -1154,7 +1157,7 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D37" t="str">
         <f>B37</f>
@@ -1174,8 +1177,8 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1226,7 +1229,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>
@@ -1235,10 +1238,10 @@
         <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
@@ -1246,7 +1249,7 @@
         <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
@@ -1254,26 +1257,26 @@
         <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
         <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
@@ -1281,7 +1284,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
         <v>21</v>
@@ -1289,56 +1292,57 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B12" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="B12" s="3"/>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>91</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>95</v>
+      </c>
+      <c r="G12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>96</v>
+      </c>
+      <c r="G13" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="D14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
@@ -1346,13 +1350,13 @@
         <v>11</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
@@ -1360,121 +1364,121 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B17" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H17" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I17" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H20" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I20" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F21" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F22" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F23" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F24" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="F25" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.45">
@@ -1752,18 +1756,18 @@
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B47" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="F47" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B48" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="F48" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>